<commit_message>
deleted some debugging code
</commit_message>
<xml_diff>
--- a/spreadsheets/Archives/OldForms/last3PForm.xlsx
+++ b/spreadsheets/Archives/OldForms/last3PForm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18975" windowHeight="5070" xr2:uid="{57EDF055-BAB1-4C42-93AB-3EA25BD5E32C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18975" windowHeight="5070" xr2:uid="{D9B333F7-2BA8-43EA-A190-7823AA40DF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,7 +261,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7664006B-9B78-46BB-9CED-6DF1E7E9DF5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{789E4836-E647-4D53-B64C-5615EA3C3A3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -595,7 +595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A1859B-A0AB-4C92-8B9B-3CAC6BB90B87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776E9DFA-5D95-4B11-81DA-EB0363AD1901}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T53"/>
   <sheetViews>

</xml_diff>